<commit_message>
Work on grade reports ...
</commit_message>
<xml_diff>
--- a/TESTDATA/testing/Noten_2/Noten_11-Gym.xlsx
+++ b/TESTDATA/testing/Noten_2/Noten_11-Gym.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="79">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4+</t>
   </si>
   <si>
     <t xml:space="preserve">6</t>
@@ -535,7 +538,7 @@
   <dimension ref="A1:V50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R7" activeCellId="0" sqref="R7"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -850,30 +853,32 @@
       <c r="G9" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="16"/>
+      <c r="H9" s="16" t="s">
+        <v>66</v>
+      </c>
       <c r="I9" s="16" t="s">
         <v>65</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L9" s="16" t="s">
         <v>16</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N9" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O9" s="16" t="s">
         <v>16</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Q9" s="16" t="s">
         <v>63</v>
@@ -888,7 +893,7 @@
         <v>16</v>
       </c>
       <c r="U9" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="V9" s="16" t="s">
         <v>16</v>
@@ -896,10 +901,10 @@
     </row>
     <row r="10" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>62</v>
@@ -912,10 +917,10 @@
         <v>16</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I10" s="16" t="s">
         <v>65</v>
@@ -924,34 +929,34 @@
         <v>16</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M10" s="16" t="s">
         <v>65</v>
       </c>
       <c r="N10" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O10" s="16" t="s">
         <v>65</v>
       </c>
       <c r="P10" s="16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Q10" s="16" t="s">
         <v>16</v>
       </c>
       <c r="R10" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="S10" s="16" t="s">
         <v>16</v>
       </c>
       <c r="T10" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="U10" s="16" t="s">
         <v>16</v>
@@ -962,10 +967,10 @@
     </row>
     <row r="11" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>62</v>
@@ -975,16 +980,16 @@
         <v>63</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G11" s="16" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J11" s="16" t="s">
         <v>63</v>
@@ -993,22 +998,22 @@
         <v>16</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N11" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O11" s="16" t="s">
         <v>16</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Q11" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R11" s="16" t="s">
         <v>16</v>
@@ -1017,7 +1022,7 @@
         <v>16</v>
       </c>
       <c r="T11" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="U11" s="16" t="s">
         <v>63</v>
@@ -1028,10 +1033,10 @@
     </row>
     <row r="12" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>62</v>
@@ -1050,28 +1055,28 @@
         <v>16</v>
       </c>
       <c r="I12" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J12" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>67</v>
-      </c>
       <c r="N12" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Q12" s="16" t="s">
         <v>63</v>

</xml_diff>